<commit_message>
updated font size, included side bar for filtering, updated to latest taxonomy version, included feedback form
</commit_message>
<xml_diff>
--- a/taxonomy_update_v1p3.xlsx
+++ b/taxonomy_update_v1p3.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iiasahub.sharepoint.com/sites/eceprog/Shared Documents/Projects/CWF/SCIL_2024/Taxonomy/Taxonomy update/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\python\scripts\streamlit_taxonomy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="847" documentId="8_{6634FA7B-39D3-4228-94A2-B46BAF2FA5EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{42EC5BBF-B574-481B-963A-A9224948EC4E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1EAF22D-9D79-4E67-979D-A206424D013F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="450" windowWidth="25440" windowHeight="15390" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7983" uniqueCount="2752">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7983" uniqueCount="2751">
   <si>
     <t>Representative Key Risk (RKR)</t>
   </si>
@@ -8457,9 +8457,6 @@
   </si>
   <si>
     <t>Chronic increases in solar radiation</t>
-  </si>
-  <si>
-    <t>Change in climagte extremes</t>
   </si>
   <si>
     <t>Coastal vegetation and marine ecosystems</t>
@@ -9516,6 +9513,21 @@
     <xf numFmtId="0" fontId="23" fillId="35" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -9541,21 +9553,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -10500,7 +10497,7 @@
         <v>28</v>
       </c>
       <c r="C35" s="81" t="s">
-        <v>2750</v>
+        <v>2749</v>
       </c>
       <c r="D35" s="81"/>
       <c r="E35" s="69"/>
@@ -10577,13 +10574,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AB1248"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="R13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="4" topLeftCell="D17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="S76" sqref="S76"/>
+      <selection pane="bottomRight" activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" customHeight="1"/>
@@ -10623,45 +10621,45 @@
       <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="124" t="s">
+      <c r="B1" s="129" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="124"/>
-      <c r="D1" s="126" t="s">
+      <c r="C1" s="129"/>
+      <c r="D1" s="131" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="126"/>
-      <c r="F1" s="126"/>
-      <c r="G1" s="126"/>
-      <c r="H1" s="126"/>
-      <c r="I1" s="125" t="s">
+      <c r="E1" s="131"/>
+      <c r="F1" s="131"/>
+      <c r="G1" s="131"/>
+      <c r="H1" s="131"/>
+      <c r="I1" s="130" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="125"/>
-      <c r="K1" s="125"/>
-      <c r="L1" s="125"/>
-      <c r="M1" s="125"/>
-      <c r="N1" s="125"/>
-      <c r="O1" s="125"/>
-      <c r="P1" s="125"/>
-      <c r="Q1" s="125"/>
-      <c r="R1" s="125"/>
-      <c r="S1" s="126" t="s">
+      <c r="J1" s="130"/>
+      <c r="K1" s="130"/>
+      <c r="L1" s="130"/>
+      <c r="M1" s="130"/>
+      <c r="N1" s="130"/>
+      <c r="O1" s="130"/>
+      <c r="P1" s="130"/>
+      <c r="Q1" s="130"/>
+      <c r="R1" s="130"/>
+      <c r="S1" s="131" t="s">
         <v>4</v>
       </c>
-      <c r="T1" s="126"/>
-      <c r="U1" s="126"/>
-      <c r="V1" s="126"/>
-      <c r="W1" s="125" t="s">
+      <c r="T1" s="131"/>
+      <c r="U1" s="131"/>
+      <c r="V1" s="131"/>
+      <c r="W1" s="130" t="s">
         <v>5</v>
       </c>
-      <c r="X1" s="125"/>
-      <c r="Y1" s="133" t="s">
+      <c r="X1" s="130"/>
+      <c r="Y1" s="124" t="s">
         <v>6</v>
       </c>
-      <c r="Z1" s="133"/>
-      <c r="AA1" s="133"/>
-      <c r="AB1" s="133"/>
+      <c r="Z1" s="124"/>
+      <c r="AA1" s="124"/>
+      <c r="AB1" s="124"/>
     </row>
     <row r="2" spans="1:28" s="2" customFormat="1" ht="18.75" customHeight="1">
       <c r="A2" s="31"/>
@@ -10672,76 +10670,76 @@
       <c r="F2" s="65"/>
       <c r="G2" s="65"/>
       <c r="H2" s="64"/>
-      <c r="I2" s="130" t="s">
+      <c r="I2" s="135" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="130"/>
-      <c r="K2" s="130"/>
-      <c r="L2" s="130"/>
-      <c r="M2" s="131" t="s">
+      <c r="J2" s="135"/>
+      <c r="K2" s="135"/>
+      <c r="L2" s="135"/>
+      <c r="M2" s="136" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="131"/>
-      <c r="O2" s="131"/>
-      <c r="P2" s="131"/>
+      <c r="N2" s="136"/>
+      <c r="O2" s="136"/>
+      <c r="P2" s="136"/>
       <c r="Q2" s="61"/>
-      <c r="R2" s="137" t="s">
+      <c r="R2" s="128" t="s">
         <v>9</v>
       </c>
-      <c r="S2" s="136" t="s">
+      <c r="S2" s="127" t="s">
         <v>10</v>
       </c>
-      <c r="T2" s="136"/>
-      <c r="U2" s="136"/>
+      <c r="T2" s="127"/>
+      <c r="U2" s="127"/>
       <c r="V2" s="60"/>
       <c r="W2" s="34"/>
       <c r="X2" s="34"/>
-      <c r="Y2" s="134" t="s">
+      <c r="Y2" s="125" t="s">
         <v>11</v>
       </c>
-      <c r="Z2" s="134"/>
-      <c r="AA2" s="134" t="s">
+      <c r="Z2" s="125"/>
+      <c r="AA2" s="125" t="s">
         <v>12</v>
       </c>
-      <c r="AB2" s="134"/>
+      <c r="AB2" s="125"/>
     </row>
     <row r="3" spans="1:28" s="35" customFormat="1" ht="19.5" customHeight="1">
       <c r="A3" s="45"/>
       <c r="B3" s="36"/>
       <c r="C3" s="36"/>
-      <c r="D3" s="135" t="s">
+      <c r="D3" s="126" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="135"/>
-      <c r="F3" s="132" t="s">
+      <c r="E3" s="126"/>
+      <c r="F3" s="137" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="132"/>
+      <c r="G3" s="137"/>
       <c r="H3" s="64"/>
       <c r="I3" s="46"/>
-      <c r="J3" s="127" t="s">
+      <c r="J3" s="132" t="s">
         <v>2660</v>
       </c>
-      <c r="K3" s="128"/>
-      <c r="L3" s="128"/>
+      <c r="K3" s="133"/>
+      <c r="L3" s="133"/>
       <c r="M3" s="46"/>
-      <c r="N3" s="129" t="s">
+      <c r="N3" s="134" t="s">
         <v>2660</v>
       </c>
-      <c r="O3" s="128"/>
-      <c r="P3" s="128"/>
+      <c r="O3" s="133"/>
+      <c r="P3" s="133"/>
       <c r="Q3" s="57"/>
-      <c r="R3" s="137"/>
-      <c r="S3" s="136"/>
-      <c r="T3" s="136"/>
-      <c r="U3" s="136"/>
+      <c r="R3" s="128"/>
+      <c r="S3" s="127"/>
+      <c r="T3" s="127"/>
+      <c r="U3" s="127"/>
       <c r="V3" s="60"/>
       <c r="W3" s="36"/>
       <c r="X3" s="36"/>
-      <c r="Y3" s="134"/>
-      <c r="Z3" s="134"/>
-      <c r="AA3" s="134"/>
-      <c r="AB3" s="134"/>
+      <c r="Y3" s="125"/>
+      <c r="Z3" s="125"/>
+      <c r="AA3" s="125"/>
+      <c r="AB3" s="125"/>
     </row>
     <row r="4" spans="1:28" s="2" customFormat="1" ht="53.65" customHeight="1">
       <c r="A4" s="38" t="s">
@@ -10829,7 +10827,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:28" ht="53.65" customHeight="1">
+    <row r="5" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A5" s="4" t="s">
         <v>31</v>
       </c>
@@ -10915,7 +10913,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="6" spans="1:28" ht="53.65" customHeight="1">
+    <row r="6" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A6" s="4" t="s">
         <v>31</v>
       </c>
@@ -11001,7 +10999,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:28" ht="53.65" customHeight="1">
+    <row r="7" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A7" s="4" t="s">
         <v>31</v>
       </c>
@@ -11087,7 +11085,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="53.65" customHeight="1">
+    <row r="8" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A8" s="4" t="s">
         <v>31</v>
       </c>
@@ -11173,7 +11171,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="9" spans="1:28" ht="53.65" customHeight="1">
+    <row r="9" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A9" s="4" t="s">
         <v>31</v>
       </c>
@@ -11259,7 +11257,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="10" spans="1:28" ht="53.65" customHeight="1">
+    <row r="10" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A10" s="4" t="s">
         <v>31</v>
       </c>
@@ -11345,7 +11343,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="11" spans="1:28" ht="53.65" customHeight="1">
+    <row r="11" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A11" s="4" t="s">
         <v>31</v>
       </c>
@@ -11431,7 +11429,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="12" spans="1:28" ht="53.65" customHeight="1">
+    <row r="12" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A12" s="4" t="s">
         <v>31</v>
       </c>
@@ -11517,7 +11515,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="13" spans="1:28" ht="53.65" customHeight="1">
+    <row r="13" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A13" s="4" t="s">
         <v>31</v>
       </c>
@@ -11603,7 +11601,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="14" spans="1:28" ht="53.65" customHeight="1">
+    <row r="14" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A14" s="4" t="s">
         <v>31</v>
       </c>
@@ -11689,7 +11687,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="15" spans="1:28" ht="53.65" customHeight="1">
+    <row r="15" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A15" s="4" t="s">
         <v>31</v>
       </c>
@@ -11775,7 +11773,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="16" spans="1:28" ht="53.65" customHeight="1">
+    <row r="16" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A16" s="4" t="s">
         <v>31</v>
       </c>
@@ -11861,7 +11859,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="17" spans="1:28" ht="53.65" customHeight="1">
+    <row r="17" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A17" s="4" t="s">
         <v>31</v>
       </c>
@@ -11947,7 +11945,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="18" spans="1:28" ht="53.65" customHeight="1">
+    <row r="18" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A18" s="4" t="s">
         <v>31</v>
       </c>
@@ -12056,10 +12054,10 @@
         <v>2684</v>
       </c>
       <c r="H19" s="23" t="s">
+        <v>2581</v>
+      </c>
+      <c r="I19" s="23" t="s">
         <v>2687</v>
-      </c>
-      <c r="I19" s="23" t="s">
-        <v>2688</v>
       </c>
       <c r="J19" s="41" t="s">
         <v>39</v>
@@ -12119,7 +12117,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="20" spans="1:28" ht="53.65" customHeight="1">
+    <row r="20" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A20" s="4" t="s">
         <v>31</v>
       </c>
@@ -12145,13 +12143,13 @@
         <v>2580</v>
       </c>
       <c r="I20" s="23" t="s">
-        <v>2689</v>
+        <v>2688</v>
       </c>
       <c r="J20" s="41" t="s">
         <v>39</v>
       </c>
       <c r="K20" s="41" t="s">
-        <v>2690</v>
+        <v>2689</v>
       </c>
       <c r="L20" s="23" t="s">
         <v>211</v>
@@ -12205,7 +12203,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:28" ht="53.65" customHeight="1">
+    <row r="21" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A21" s="4" t="s">
         <v>31</v>
       </c>
@@ -12231,13 +12229,13 @@
         <v>2580</v>
       </c>
       <c r="I21" s="23" t="s">
-        <v>2691</v>
+        <v>2690</v>
       </c>
       <c r="J21" s="41" t="s">
         <v>39</v>
       </c>
       <c r="K21" s="41" t="s">
-        <v>2692</v>
+        <v>2691</v>
       </c>
       <c r="L21" s="23" t="s">
         <v>39</v>
@@ -12291,7 +12289,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:28" ht="53.65" customHeight="1">
+    <row r="22" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A22" s="4" t="s">
         <v>31</v>
       </c>
@@ -12311,13 +12309,13 @@
         <v>245</v>
       </c>
       <c r="G22" s="21" t="s">
-        <v>2693</v>
+        <v>2692</v>
       </c>
       <c r="H22" s="114" t="s">
         <v>2581</v>
       </c>
       <c r="I22" s="23" t="s">
-        <v>2699</v>
+        <v>2698</v>
       </c>
       <c r="J22" s="41" t="s">
         <v>131</v>
@@ -12377,7 +12375,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:28" ht="53.65" customHeight="1">
+    <row r="23" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A23" s="4" t="s">
         <v>31</v>
       </c>
@@ -12397,19 +12395,19 @@
         <v>164</v>
       </c>
       <c r="G23" s="21" t="s">
-        <v>2694</v>
+        <v>2693</v>
       </c>
       <c r="H23" s="114" t="s">
         <v>2581</v>
       </c>
       <c r="I23" s="23" t="s">
-        <v>2700</v>
+        <v>2699</v>
       </c>
       <c r="J23" s="23" t="s">
         <v>131</v>
       </c>
       <c r="K23" s="23" t="s">
-        <v>2701</v>
+        <v>2700</v>
       </c>
       <c r="L23" s="23" t="s">
         <v>39</v>
@@ -12463,7 +12461,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:28" ht="53.65" customHeight="1">
+    <row r="24" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A24" s="4" t="s">
         <v>31</v>
       </c>
@@ -12483,13 +12481,13 @@
         <v>267</v>
       </c>
       <c r="G24" s="21" t="s">
-        <v>2695</v>
+        <v>2694</v>
       </c>
       <c r="H24" s="114" t="s">
         <v>2580</v>
       </c>
       <c r="I24" s="23" t="s">
-        <v>2702</v>
+        <v>2701</v>
       </c>
       <c r="J24" s="41" t="s">
         <v>39</v>
@@ -12549,7 +12547,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:28" ht="53.65" customHeight="1">
+    <row r="25" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A25" s="4" t="s">
         <v>31</v>
       </c>
@@ -12569,19 +12567,19 @@
         <v>37</v>
       </c>
       <c r="G25" s="21" t="s">
-        <v>2696</v>
+        <v>2695</v>
       </c>
       <c r="H25" s="114" t="s">
         <v>2580</v>
       </c>
       <c r="I25" s="23" t="s">
-        <v>2703</v>
+        <v>2702</v>
       </c>
       <c r="J25" s="23" t="s">
         <v>39</v>
       </c>
       <c r="K25" s="23" t="s">
-        <v>2704</v>
+        <v>2703</v>
       </c>
       <c r="L25" s="23" t="s">
         <v>133</v>
@@ -12635,7 +12633,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:28" ht="53.65" customHeight="1">
+    <row r="26" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A26" s="4" t="s">
         <v>31</v>
       </c>
@@ -12655,13 +12653,13 @@
         <v>245</v>
       </c>
       <c r="G26" s="21" t="s">
-        <v>2697</v>
+        <v>2696</v>
       </c>
       <c r="H26" s="114" t="s">
         <v>2581</v>
       </c>
       <c r="I26" s="23" t="s">
-        <v>2705</v>
+        <v>2704</v>
       </c>
       <c r="J26" s="23" t="s">
         <v>39</v>
@@ -12721,7 +12719,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:28" ht="53.65" customHeight="1">
+    <row r="27" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A27" s="4" t="s">
         <v>31</v>
       </c>
@@ -12741,13 +12739,13 @@
         <v>37</v>
       </c>
       <c r="G27" s="21" t="s">
-        <v>2698</v>
+        <v>2697</v>
       </c>
       <c r="H27" s="114" t="s">
         <v>2580</v>
       </c>
       <c r="I27" s="23" t="s">
-        <v>2706</v>
+        <v>2705</v>
       </c>
       <c r="J27" s="23" t="s">
         <v>39</v>
@@ -12807,7 +12805,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="1:28" ht="53.65" customHeight="1">
+    <row r="28" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A28" s="4" t="s">
         <v>31</v>
       </c>
@@ -12827,13 +12825,13 @@
         <v>312</v>
       </c>
       <c r="G28" s="21" t="s">
-        <v>2707</v>
+        <v>2706</v>
       </c>
       <c r="H28" s="114" t="s">
         <v>2580</v>
       </c>
       <c r="I28" s="23" t="s">
-        <v>2715</v>
+        <v>2714</v>
       </c>
       <c r="J28" s="23" t="s">
         <v>39</v>
@@ -12893,7 +12891,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="29" spans="1:28" ht="53.65" customHeight="1">
+    <row r="29" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A29" s="4" t="s">
         <v>31</v>
       </c>
@@ -12913,13 +12911,13 @@
         <v>37</v>
       </c>
       <c r="G29" s="21" t="s">
-        <v>2708</v>
+        <v>2707</v>
       </c>
       <c r="H29" s="114" t="s">
         <v>2580</v>
       </c>
       <c r="I29" s="23" t="s">
-        <v>2716</v>
+        <v>2715</v>
       </c>
       <c r="J29" s="23" t="s">
         <v>39</v>
@@ -12979,7 +12977,7 @@
         <v>2117</v>
       </c>
     </row>
-    <row r="30" spans="1:28" ht="53.65" customHeight="1">
+    <row r="30" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A30" s="4" t="s">
         <v>31</v>
       </c>
@@ -12999,19 +12997,19 @@
         <v>60</v>
       </c>
       <c r="G30" s="21" t="s">
-        <v>2709</v>
+        <v>2708</v>
       </c>
       <c r="H30" s="114" t="s">
         <v>2581</v>
       </c>
       <c r="I30" s="23" t="s">
-        <v>2717</v>
+        <v>2716</v>
       </c>
       <c r="J30" s="41" t="s">
         <v>39</v>
       </c>
       <c r="K30" s="41" t="s">
-        <v>2718</v>
+        <v>2717</v>
       </c>
       <c r="L30" s="23" t="s">
         <v>39</v>
@@ -13065,7 +13063,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:28" ht="53.65" customHeight="1">
+    <row r="31" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A31" s="4" t="s">
         <v>31</v>
       </c>
@@ -13085,19 +13083,19 @@
         <v>164</v>
       </c>
       <c r="G31" s="21" t="s">
-        <v>2710</v>
+        <v>2709</v>
       </c>
       <c r="H31" s="114" t="s">
         <v>2581</v>
       </c>
       <c r="I31" s="23" t="s">
-        <v>2719</v>
+        <v>2718</v>
       </c>
       <c r="J31" s="41" t="s">
         <v>39</v>
       </c>
       <c r="K31" s="41" t="s">
-        <v>2718</v>
+        <v>2717</v>
       </c>
       <c r="L31" s="23" t="s">
         <v>39</v>
@@ -13151,7 +13149,7 @@
         <v>2582</v>
       </c>
     </row>
-    <row r="32" spans="1:28" ht="53.65" customHeight="1">
+    <row r="32" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A32" s="4" t="s">
         <v>31</v>
       </c>
@@ -13171,13 +13169,13 @@
         <v>312</v>
       </c>
       <c r="G32" s="21" t="s">
-        <v>2711</v>
+        <v>2710</v>
       </c>
       <c r="H32" s="114" t="s">
         <v>2580</v>
       </c>
       <c r="I32" s="23" t="s">
-        <v>2720</v>
+        <v>2719</v>
       </c>
       <c r="J32" s="23" t="s">
         <v>39</v>
@@ -13237,7 +13235,7 @@
         <v>2583</v>
       </c>
     </row>
-    <row r="33" spans="1:28" ht="53.65" customHeight="1">
+    <row r="33" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A33" s="4" t="s">
         <v>31</v>
       </c>
@@ -13257,13 +13255,13 @@
         <v>164</v>
       </c>
       <c r="G33" s="21" t="s">
-        <v>2712</v>
+        <v>2711</v>
       </c>
       <c r="H33" s="114" t="s">
         <v>2581</v>
       </c>
       <c r="I33" s="23" t="s">
-        <v>2721</v>
+        <v>2720</v>
       </c>
       <c r="J33" s="23" t="s">
         <v>39</v>
@@ -13323,7 +13321,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:28" ht="53.65" customHeight="1">
+    <row r="34" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A34" s="4" t="s">
         <v>31</v>
       </c>
@@ -13343,19 +13341,19 @@
         <v>37</v>
       </c>
       <c r="G34" s="21" t="s">
-        <v>2713</v>
+        <v>2712</v>
       </c>
       <c r="H34" s="114" t="s">
         <v>2580</v>
       </c>
       <c r="I34" s="23" t="s">
-        <v>2722</v>
+        <v>2721</v>
       </c>
       <c r="J34" s="23" t="s">
         <v>39</v>
       </c>
       <c r="K34" s="23" t="s">
-        <v>2723</v>
+        <v>2722</v>
       </c>
       <c r="L34" s="23" t="s">
         <v>132</v>
@@ -13409,7 +13407,7 @@
         <v>2117</v>
       </c>
     </row>
-    <row r="35" spans="1:28" ht="53.65" customHeight="1">
+    <row r="35" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A35" s="4" t="s">
         <v>31</v>
       </c>
@@ -13429,19 +13427,19 @@
         <v>164</v>
       </c>
       <c r="G35" s="21" t="s">
-        <v>2714</v>
+        <v>2713</v>
       </c>
       <c r="H35" s="114" t="s">
         <v>2581</v>
       </c>
       <c r="I35" s="23" t="s">
-        <v>2724</v>
+        <v>2723</v>
       </c>
       <c r="J35" s="41" t="s">
         <v>39</v>
       </c>
       <c r="K35" s="41" t="s">
-        <v>2723</v>
+        <v>2722</v>
       </c>
       <c r="L35" s="23" t="s">
         <v>132</v>
@@ -13495,7 +13493,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="36" spans="1:28" ht="53.65" customHeight="1">
+    <row r="36" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A36" s="4" t="s">
         <v>31</v>
       </c>
@@ -13515,19 +13513,19 @@
         <v>37</v>
       </c>
       <c r="G36" s="21" t="s">
-        <v>2725</v>
+        <v>2724</v>
       </c>
       <c r="H36" s="114" t="s">
         <v>2580</v>
       </c>
       <c r="I36" s="23" t="s">
-        <v>2729</v>
+        <v>2728</v>
       </c>
       <c r="J36" s="23" t="s">
         <v>131</v>
       </c>
       <c r="K36" s="23" t="s">
-        <v>2730</v>
+        <v>2729</v>
       </c>
       <c r="L36" s="23" t="s">
         <v>39</v>
@@ -13581,7 +13579,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="37" spans="1:28" ht="53.65" customHeight="1">
+    <row r="37" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A37" s="4" t="s">
         <v>31</v>
       </c>
@@ -13601,19 +13599,19 @@
         <v>164</v>
       </c>
       <c r="G37" s="21" t="s">
-        <v>2726</v>
+        <v>2725</v>
       </c>
       <c r="H37" s="114" t="s">
         <v>2581</v>
       </c>
       <c r="I37" s="23" t="s">
-        <v>2731</v>
+        <v>2730</v>
       </c>
       <c r="J37" s="23" t="s">
         <v>39</v>
       </c>
       <c r="K37" s="23" t="s">
-        <v>2732</v>
+        <v>2731</v>
       </c>
       <c r="L37" s="23" t="s">
         <v>39</v>
@@ -13667,7 +13665,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="38" spans="1:28" ht="53.65" customHeight="1">
+    <row r="38" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A38" s="4" t="s">
         <v>31</v>
       </c>
@@ -13687,13 +13685,13 @@
         <v>164</v>
       </c>
       <c r="G38" s="21" t="s">
-        <v>2727</v>
+        <v>2726</v>
       </c>
       <c r="H38" s="114" t="s">
         <v>2581</v>
       </c>
       <c r="I38" s="23" t="s">
-        <v>2733</v>
+        <v>2732</v>
       </c>
       <c r="J38" s="23" t="s">
         <v>369</v>
@@ -13753,7 +13751,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="39" spans="1:28" ht="53.65" customHeight="1">
+    <row r="39" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A39" s="4" t="s">
         <v>31</v>
       </c>
@@ -13773,13 +13771,13 @@
         <v>164</v>
       </c>
       <c r="G39" s="21" t="s">
-        <v>2728</v>
+        <v>2727</v>
       </c>
       <c r="H39" s="114" t="s">
         <v>2581</v>
       </c>
       <c r="I39" s="23" t="s">
-        <v>2734</v>
+        <v>2733</v>
       </c>
       <c r="J39" s="23" t="s">
         <v>39</v>
@@ -13839,7 +13837,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="40" spans="1:28" ht="53.65" customHeight="1">
+    <row r="40" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A40" s="7" t="s">
         <v>443</v>
       </c>
@@ -13865,7 +13863,7 @@
         <v>2580</v>
       </c>
       <c r="I40" s="52" t="s">
-        <v>2739</v>
+        <v>2738</v>
       </c>
       <c r="J40" s="53" t="s">
         <v>39</v>
@@ -13925,7 +13923,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="41" spans="1:28" ht="53.65" customHeight="1">
+    <row r="41" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A41" s="7" t="s">
         <v>443</v>
       </c>
@@ -13945,13 +13943,13 @@
         <v>60</v>
       </c>
       <c r="G41" s="52" t="s">
-        <v>2735</v>
+        <v>2734</v>
       </c>
       <c r="H41" s="51" t="s">
         <v>2581</v>
       </c>
       <c r="I41" s="52" t="s">
-        <v>2740</v>
+        <v>2739</v>
       </c>
       <c r="J41" s="53" t="s">
         <v>39</v>
@@ -13981,7 +13979,7 @@
         <v>67</v>
       </c>
       <c r="S41" s="2" t="s">
-        <v>2751</v>
+        <v>2750</v>
       </c>
       <c r="T41" s="2" t="s">
         <v>454</v>
@@ -14011,7 +14009,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="42" spans="1:28" ht="53.65" customHeight="1">
+    <row r="42" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A42" s="7" t="s">
         <v>443</v>
       </c>
@@ -14031,13 +14029,13 @@
         <v>60</v>
       </c>
       <c r="G42" s="52" t="s">
-        <v>2736</v>
+        <v>2735</v>
       </c>
       <c r="H42" s="51" t="s">
         <v>2581</v>
       </c>
       <c r="I42" s="52" t="s">
-        <v>2741</v>
+        <v>2740</v>
       </c>
       <c r="J42" s="53" t="s">
         <v>39</v>
@@ -14097,7 +14095,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="43" spans="1:28" ht="53.65" customHeight="1">
+    <row r="43" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A43" s="7" t="s">
         <v>443</v>
       </c>
@@ -14117,13 +14115,13 @@
         <v>37</v>
       </c>
       <c r="G43" s="52" t="s">
-        <v>2737</v>
+        <v>2736</v>
       </c>
       <c r="H43" s="51" t="s">
         <v>2580</v>
       </c>
       <c r="I43" s="52" t="s">
-        <v>2742</v>
+        <v>2741</v>
       </c>
       <c r="J43" s="53" t="s">
         <v>39</v>
@@ -14183,7 +14181,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="44" spans="1:28" ht="53.65" customHeight="1">
+    <row r="44" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A44" s="7" t="s">
         <v>443</v>
       </c>
@@ -14203,13 +14201,13 @@
         <v>112</v>
       </c>
       <c r="G44" s="52" t="s">
-        <v>2738</v>
+        <v>2737</v>
       </c>
       <c r="H44" s="51" t="s">
         <v>2580</v>
       </c>
       <c r="I44" s="52" t="s">
-        <v>2743</v>
+        <v>2742</v>
       </c>
       <c r="J44" s="53" t="s">
         <v>39</v>
@@ -14269,7 +14267,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="45" spans="1:28" ht="53.65" customHeight="1">
+    <row r="45" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A45" s="7" t="s">
         <v>443</v>
       </c>
@@ -14289,19 +14287,19 @@
         <v>60</v>
       </c>
       <c r="G45" s="22" t="s">
-        <v>2744</v>
+        <v>2743</v>
       </c>
       <c r="H45" s="114" t="s">
         <v>2581</v>
       </c>
       <c r="I45" s="41" t="s">
-        <v>2746</v>
+        <v>2745</v>
       </c>
       <c r="J45" s="41" t="s">
         <v>131</v>
       </c>
       <c r="K45" s="41" t="s">
-        <v>2747</v>
+        <v>2746</v>
       </c>
       <c r="L45" s="23" t="s">
         <v>478</v>
@@ -14355,7 +14353,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="46" spans="1:28" ht="53.65" customHeight="1">
+    <row r="46" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A46" s="7" t="s">
         <v>443</v>
       </c>
@@ -14375,19 +14373,19 @@
         <v>60</v>
       </c>
       <c r="G46" s="22" t="s">
-        <v>2745</v>
+        <v>2744</v>
       </c>
       <c r="H46" s="114" t="s">
         <v>2581</v>
       </c>
       <c r="I46" s="41" t="s">
-        <v>2748</v>
+        <v>2747</v>
       </c>
       <c r="J46" s="43" t="s">
         <v>39</v>
       </c>
       <c r="K46" s="41" t="s">
-        <v>2749</v>
+        <v>2748</v>
       </c>
       <c r="L46" s="23" t="s">
         <v>485</v>
@@ -14441,7 +14439,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="47" spans="1:28" ht="53.65" customHeight="1">
+    <row r="47" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A47" s="7" t="s">
         <v>443</v>
       </c>
@@ -14527,7 +14525,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="48" spans="1:28" ht="53.65" customHeight="1">
+    <row r="48" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A48" s="7" t="s">
         <v>443</v>
       </c>
@@ -14613,7 +14611,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="49" spans="1:28" ht="53.65" customHeight="1">
+    <row r="49" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A49" s="7" t="s">
         <v>443</v>
       </c>
@@ -14699,7 +14697,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="50" spans="1:28" ht="53.65" customHeight="1">
+    <row r="50" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A50" s="7" t="s">
         <v>443</v>
       </c>
@@ -14785,7 +14783,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="51" spans="1:28" ht="53.65" customHeight="1">
+    <row r="51" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A51" s="7" t="s">
         <v>443</v>
       </c>
@@ -14871,7 +14869,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="52" spans="1:28" ht="53.65" customHeight="1">
+    <row r="52" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A52" s="7" t="s">
         <v>443</v>
       </c>
@@ -14957,7 +14955,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="53" spans="1:28" ht="53.65" customHeight="1">
+    <row r="53" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A53" s="7" t="s">
         <v>443</v>
       </c>
@@ -15043,7 +15041,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="54" spans="1:28" ht="53.65" customHeight="1">
+    <row r="54" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A54" s="7" t="s">
         <v>443</v>
       </c>
@@ -15129,7 +15127,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="55" spans="1:28" ht="53.65" customHeight="1">
+    <row r="55" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A55" s="7" t="s">
         <v>443</v>
       </c>
@@ -15215,7 +15213,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="56" spans="1:28" ht="53.65" customHeight="1">
+    <row r="56" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A56" s="7" t="s">
         <v>443</v>
       </c>
@@ -15301,7 +15299,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="57" spans="1:28" ht="53.65" customHeight="1">
+    <row r="57" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A57" s="7" t="s">
         <v>443</v>
       </c>
@@ -15387,7 +15385,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="58" spans="1:28" ht="53.65" customHeight="1">
+    <row r="58" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A58" s="7" t="s">
         <v>443</v>
       </c>
@@ -15473,7 +15471,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="59" spans="1:28" ht="53.65" customHeight="1">
+    <row r="59" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A59" s="7" t="s">
         <v>443</v>
       </c>
@@ -15559,7 +15557,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="60" spans="1:28" ht="53.65" customHeight="1">
+    <row r="60" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A60" s="7" t="s">
         <v>443</v>
       </c>
@@ -15645,7 +15643,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="61" spans="1:28" ht="53.65" customHeight="1">
+    <row r="61" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A61" s="7" t="s">
         <v>443</v>
       </c>
@@ -15731,7 +15729,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="62" spans="1:28" ht="53.65" customHeight="1">
+    <row r="62" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A62" s="7" t="s">
         <v>443</v>
       </c>
@@ -15817,7 +15815,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="63" spans="1:28" ht="53.65" customHeight="1">
+    <row r="63" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A63" s="7" t="s">
         <v>443</v>
       </c>
@@ -15903,7 +15901,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="64" spans="1:28" ht="53.65" customHeight="1">
+    <row r="64" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A64" s="7" t="s">
         <v>443</v>
       </c>
@@ -15989,7 +15987,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="65" spans="1:28" ht="53.65" customHeight="1">
+    <row r="65" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A65" s="7" t="s">
         <v>443</v>
       </c>
@@ -16075,7 +16073,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="66" spans="1:28" ht="53.65" customHeight="1">
+    <row r="66" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A66" s="7" t="s">
         <v>443</v>
       </c>
@@ -16161,7 +16159,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="67" spans="1:28" ht="53.65" customHeight="1">
+    <row r="67" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A67" s="7" t="s">
         <v>443</v>
       </c>
@@ -16247,7 +16245,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="68" spans="1:28" ht="53.65" customHeight="1">
+    <row r="68" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A68" s="7" t="s">
         <v>443</v>
       </c>
@@ -16333,7 +16331,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="69" spans="1:28" ht="53.65" customHeight="1">
+    <row r="69" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A69" s="7" t="s">
         <v>443</v>
       </c>
@@ -16419,7 +16417,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="70" spans="1:28" ht="53.65" customHeight="1">
+    <row r="70" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A70" s="7" t="s">
         <v>443</v>
       </c>
@@ -16505,7 +16503,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="71" spans="1:28" ht="53.65" customHeight="1">
+    <row r="71" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A71" s="7" t="s">
         <v>443</v>
       </c>
@@ -16591,7 +16589,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="72" spans="1:28" ht="53.65" customHeight="1">
+    <row r="72" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A72" s="7" t="s">
         <v>443</v>
       </c>
@@ -16677,7 +16675,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="73" spans="1:28" ht="53.65" customHeight="1">
+    <row r="73" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A73" s="7" t="s">
         <v>443</v>
       </c>
@@ -16763,7 +16761,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="74" spans="1:28" ht="53.65" customHeight="1">
+    <row r="74" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A74" s="7" t="s">
         <v>443</v>
       </c>
@@ -16849,7 +16847,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="75" spans="1:28" ht="53.65" customHeight="1">
+    <row r="75" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A75" s="8" t="s">
         <v>757</v>
       </c>
@@ -16935,7 +16933,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="76" spans="1:28" ht="53.65" customHeight="1">
+    <row r="76" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A76" s="8" t="s">
         <v>757</v>
       </c>
@@ -17021,7 +17019,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="77" spans="1:28" ht="53.65" customHeight="1">
+    <row r="77" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A77" s="8" t="s">
         <v>757</v>
       </c>
@@ -17107,7 +17105,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="78" spans="1:28" ht="53.65" customHeight="1">
+    <row r="78" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A78" s="8" t="s">
         <v>757</v>
       </c>
@@ -17193,7 +17191,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="79" spans="1:28" ht="53.65" customHeight="1">
+    <row r="79" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A79" s="8" t="s">
         <v>757</v>
       </c>
@@ -17279,7 +17277,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="80" spans="1:28" ht="53.65" customHeight="1">
+    <row r="80" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A80" s="8" t="s">
         <v>757</v>
       </c>
@@ -17365,7 +17363,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="81" spans="1:28" ht="53.65" customHeight="1">
+    <row r="81" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A81" s="8" t="s">
         <v>757</v>
       </c>
@@ -17451,7 +17449,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="82" spans="1:28" ht="53.65" customHeight="1">
+    <row r="82" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A82" s="8" t="s">
         <v>757</v>
       </c>
@@ -17537,7 +17535,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="83" spans="1:28" ht="53.65" customHeight="1">
+    <row r="83" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A83" s="8" t="s">
         <v>757</v>
       </c>
@@ -17623,7 +17621,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="84" spans="1:28" ht="53.65" customHeight="1">
+    <row r="84" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A84" s="8" t="s">
         <v>757</v>
       </c>
@@ -17709,7 +17707,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="85" spans="1:28" ht="53.65" customHeight="1">
+    <row r="85" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A85" s="8" t="s">
         <v>757</v>
       </c>
@@ -17795,7 +17793,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="86" spans="1:28" ht="53.65" customHeight="1">
+    <row r="86" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A86" s="8" t="s">
         <v>757</v>
       </c>
@@ -17881,7 +17879,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="87" spans="1:28" ht="53.65" customHeight="1">
+    <row r="87" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A87" s="8" t="s">
         <v>757</v>
       </c>
@@ -17967,7 +17965,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="88" spans="1:28" ht="53.65" customHeight="1">
+    <row r="88" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A88" s="8" t="s">
         <v>757</v>
       </c>
@@ -18053,7 +18051,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="89" spans="1:28" ht="53.65" customHeight="1">
+    <row r="89" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A89" s="8" t="s">
         <v>757</v>
       </c>
@@ -18139,7 +18137,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="90" spans="1:28" ht="53.65" customHeight="1">
+    <row r="90" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A90" s="8" t="s">
         <v>757</v>
       </c>
@@ -18225,7 +18223,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="91" spans="1:28" ht="53.65" customHeight="1">
+    <row r="91" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A91" s="8" t="s">
         <v>757</v>
       </c>
@@ -18311,7 +18309,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="92" spans="1:28" ht="53.65" customHeight="1">
+    <row r="92" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A92" s="8" t="s">
         <v>757</v>
       </c>
@@ -18397,7 +18395,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="93" spans="1:28" ht="53.65" customHeight="1">
+    <row r="93" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A93" s="8" t="s">
         <v>757</v>
       </c>
@@ -18483,7 +18481,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="94" spans="1:28" ht="53.65" customHeight="1">
+    <row r="94" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A94" s="8" t="s">
         <v>757</v>
       </c>
@@ -18569,7 +18567,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="95" spans="1:28" ht="53.65" customHeight="1">
+    <row r="95" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A95" s="8" t="s">
         <v>757</v>
       </c>
@@ -18655,7 +18653,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="96" spans="1:28" ht="53.65" customHeight="1">
+    <row r="96" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A96" s="8" t="s">
         <v>757</v>
       </c>
@@ -18741,7 +18739,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="97" spans="1:28" ht="53.65" customHeight="1">
+    <row r="97" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A97" s="8" t="s">
         <v>757</v>
       </c>
@@ -18827,7 +18825,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="98" spans="1:28" ht="53.65" customHeight="1">
+    <row r="98" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A98" s="8" t="s">
         <v>757</v>
       </c>
@@ -18913,7 +18911,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="99" spans="1:28" ht="53.65" customHeight="1">
+    <row r="99" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A99" s="8" t="s">
         <v>757</v>
       </c>
@@ -18999,7 +18997,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="100" spans="1:28" ht="53.65" customHeight="1">
+    <row r="100" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A100" s="8" t="s">
         <v>757</v>
       </c>
@@ -19085,7 +19083,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="101" spans="1:28" ht="53.65" customHeight="1">
+    <row r="101" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A101" s="8" t="s">
         <v>757</v>
       </c>
@@ -19171,7 +19169,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="102" spans="1:28" ht="53.65" customHeight="1">
+    <row r="102" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A102" s="8" t="s">
         <v>757</v>
       </c>
@@ -19257,7 +19255,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="103" spans="1:28" ht="53.65" customHeight="1">
+    <row r="103" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A103" s="8" t="s">
         <v>757</v>
       </c>
@@ -19343,7 +19341,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="104" spans="1:28" ht="53.65" customHeight="1">
+    <row r="104" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A104" s="8" t="s">
         <v>757</v>
       </c>
@@ -19429,7 +19427,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="105" spans="1:28" ht="53.65" customHeight="1">
+    <row r="105" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A105" s="8" t="s">
         <v>757</v>
       </c>
@@ -19515,7 +19513,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="106" spans="1:28" ht="53.65" customHeight="1">
+    <row r="106" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A106" s="8" t="s">
         <v>757</v>
       </c>
@@ -19601,7 +19599,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="107" spans="1:28" ht="53.65" customHeight="1">
+    <row r="107" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A107" s="8" t="s">
         <v>757</v>
       </c>
@@ -19687,7 +19685,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="108" spans="1:28" ht="53.65" customHeight="1">
+    <row r="108" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A108" s="8" t="s">
         <v>757</v>
       </c>
@@ -19773,7 +19771,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="109" spans="1:28" ht="53.65" customHeight="1">
+    <row r="109" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A109" s="8" t="s">
         <v>757</v>
       </c>
@@ -19859,7 +19857,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="110" spans="1:28" ht="53.65" customHeight="1">
+    <row r="110" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A110" s="9" t="s">
         <v>1034</v>
       </c>
@@ -19945,7 +19943,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="111" spans="1:28" ht="53.65" customHeight="1">
+    <row r="111" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A111" s="9" t="s">
         <v>1034</v>
       </c>
@@ -20031,7 +20029,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="112" spans="1:28" ht="53.65" customHeight="1">
+    <row r="112" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A112" s="9" t="s">
         <v>1034</v>
       </c>
@@ -20117,7 +20115,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="113" spans="1:28" ht="53.65" customHeight="1">
+    <row r="113" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A113" s="9" t="s">
         <v>1034</v>
       </c>
@@ -20203,7 +20201,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="114" spans="1:28" ht="53.65" customHeight="1">
+    <row r="114" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A114" s="9" t="s">
         <v>1034</v>
       </c>
@@ -20289,7 +20287,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="115" spans="1:28" ht="53.65" customHeight="1">
+    <row r="115" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A115" s="9" t="s">
         <v>1034</v>
       </c>
@@ -20375,7 +20373,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="116" spans="1:28" ht="53.65" customHeight="1">
+    <row r="116" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A116" s="9" t="s">
         <v>1034</v>
       </c>
@@ -20461,7 +20459,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="117" spans="1:28" ht="53.65" customHeight="1">
+    <row r="117" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A117" s="9" t="s">
         <v>1034</v>
       </c>
@@ -20547,7 +20545,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="118" spans="1:28" ht="53.65" customHeight="1">
+    <row r="118" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A118" s="9" t="s">
         <v>1034</v>
       </c>
@@ -20633,7 +20631,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="119" spans="1:28" ht="53.65" customHeight="1">
+    <row r="119" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A119" s="9" t="s">
         <v>1034</v>
       </c>
@@ -20719,7 +20717,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="120" spans="1:28" ht="53.65" customHeight="1">
+    <row r="120" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A120" s="9" t="s">
         <v>1034</v>
       </c>
@@ -20805,7 +20803,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="121" spans="1:28" ht="53.65" customHeight="1">
+    <row r="121" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A121" s="9" t="s">
         <v>1034</v>
       </c>
@@ -20891,7 +20889,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="122" spans="1:28" ht="53.65" customHeight="1">
+    <row r="122" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A122" s="9" t="s">
         <v>1034</v>
       </c>
@@ -20977,7 +20975,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="123" spans="1:28" ht="53.65" customHeight="1">
+    <row r="123" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A123" s="9" t="s">
         <v>1034</v>
       </c>
@@ -21063,7 +21061,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="124" spans="1:28" ht="53.65" customHeight="1">
+    <row r="124" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A124" s="9" t="s">
         <v>1034</v>
       </c>
@@ -21149,7 +21147,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="125" spans="1:28" ht="53.65" customHeight="1">
+    <row r="125" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A125" s="9" t="s">
         <v>1034</v>
       </c>
@@ -21235,7 +21233,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="126" spans="1:28" ht="53.65" customHeight="1">
+    <row r="126" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A126" s="9" t="s">
         <v>1034</v>
       </c>
@@ -21321,7 +21319,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="127" spans="1:28" ht="53.65" customHeight="1">
+    <row r="127" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A127" s="9" t="s">
         <v>1034</v>
       </c>
@@ -21407,7 +21405,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="128" spans="1:28" ht="53.65" customHeight="1">
+    <row r="128" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A128" s="9" t="s">
         <v>1034</v>
       </c>
@@ -21493,7 +21491,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="129" spans="1:28" ht="53.65" customHeight="1">
+    <row r="129" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A129" s="9" t="s">
         <v>1034</v>
       </c>
@@ -21579,7 +21577,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="130" spans="1:28" ht="53.65" customHeight="1">
+    <row r="130" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A130" s="9" t="s">
         <v>1034</v>
       </c>
@@ -21665,7 +21663,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="131" spans="1:28" ht="53.65" customHeight="1">
+    <row r="131" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A131" s="9" t="s">
         <v>1034</v>
       </c>
@@ -21751,7 +21749,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="132" spans="1:28" ht="53.65" customHeight="1">
+    <row r="132" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A132" s="9" t="s">
         <v>1034</v>
       </c>
@@ -21837,7 +21835,7 @@
         <v>2440</v>
       </c>
     </row>
-    <row r="133" spans="1:28" ht="53.65" customHeight="1">
+    <row r="133" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A133" s="9" t="s">
         <v>1034</v>
       </c>
@@ -21923,7 +21921,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="134" spans="1:28" ht="53.65" customHeight="1">
+    <row r="134" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A134" s="9" t="s">
         <v>1034</v>
       </c>
@@ -22009,7 +22007,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="135" spans="1:28" ht="53.65" customHeight="1">
+    <row r="135" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A135" s="9" t="s">
         <v>1034</v>
       </c>
@@ -22095,7 +22093,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="136" spans="1:28" ht="53.65" customHeight="1">
+    <row r="136" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A136" s="9" t="s">
         <v>1034</v>
       </c>
@@ -22181,7 +22179,7 @@
         <v>1291</v>
       </c>
     </row>
-    <row r="137" spans="1:28" ht="53.65" customHeight="1">
+    <row r="137" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A137" s="9" t="s">
         <v>1034</v>
       </c>
@@ -22267,7 +22265,7 @@
         <v>1291</v>
       </c>
     </row>
-    <row r="138" spans="1:28" ht="53.65" customHeight="1">
+    <row r="138" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A138" s="9" t="s">
         <v>1034</v>
       </c>
@@ -22353,7 +22351,7 @@
         <v>1930</v>
       </c>
     </row>
-    <row r="139" spans="1:28" ht="53.65" customHeight="1">
+    <row r="139" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A139" s="9" t="s">
         <v>1034</v>
       </c>
@@ -22439,7 +22437,7 @@
         <v>1291</v>
       </c>
     </row>
-    <row r="140" spans="1:28" ht="53.65" customHeight="1">
+    <row r="140" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A140" s="9" t="s">
         <v>1034</v>
       </c>
@@ -22525,7 +22523,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="141" spans="1:28" ht="53.65" customHeight="1">
+    <row r="141" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A141" s="9" t="s">
         <v>1034</v>
       </c>
@@ -22611,7 +22609,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="142" spans="1:28" ht="53.65" customHeight="1">
+    <row r="142" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A142" s="9" t="s">
         <v>1034</v>
       </c>
@@ -22697,7 +22695,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="143" spans="1:28" ht="53.65" customHeight="1">
+    <row r="143" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A143" s="9" t="s">
         <v>1034</v>
       </c>
@@ -22783,7 +22781,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="144" spans="1:28" ht="53.65" customHeight="1">
+    <row r="144" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A144" s="9" t="s">
         <v>1034</v>
       </c>
@@ -22869,7 +22867,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="145" spans="1:28" ht="53.65" customHeight="1">
+    <row r="145" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A145" s="10" t="s">
         <v>1365</v>
       </c>
@@ -22955,7 +22953,7 @@
         <v>2584</v>
       </c>
     </row>
-    <row r="146" spans="1:28" ht="53.65" customHeight="1">
+    <row r="146" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A146" s="10" t="s">
         <v>1365</v>
       </c>
@@ -23041,7 +23039,7 @@
         <v>2585</v>
       </c>
     </row>
-    <row r="147" spans="1:28" ht="53.65" customHeight="1">
+    <row r="147" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A147" s="10" t="s">
         <v>1365</v>
       </c>
@@ -23127,7 +23125,7 @@
         <v>2586</v>
       </c>
     </row>
-    <row r="148" spans="1:28" ht="53.65" customHeight="1">
+    <row r="148" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A148" s="10" t="s">
         <v>1365</v>
       </c>
@@ -23213,7 +23211,7 @@
         <v>2587</v>
       </c>
     </row>
-    <row r="149" spans="1:28" ht="53.65" customHeight="1">
+    <row r="149" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A149" s="10" t="s">
         <v>1365</v>
       </c>
@@ -23299,7 +23297,7 @@
         <v>2588</v>
       </c>
     </row>
-    <row r="150" spans="1:28" ht="53.65" customHeight="1">
+    <row r="150" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A150" s="10" t="s">
         <v>1365</v>
       </c>
@@ -23385,7 +23383,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="151" spans="1:28" ht="53.65" customHeight="1">
+    <row r="151" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A151" s="10" t="s">
         <v>1365</v>
       </c>
@@ -23471,7 +23469,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="152" spans="1:28" ht="53.65" customHeight="1">
+    <row r="152" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A152" s="10" t="s">
         <v>1365</v>
       </c>
@@ -23557,7 +23555,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="153" spans="1:28" ht="53.65" customHeight="1">
+    <row r="153" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A153" s="10" t="s">
         <v>1365</v>
       </c>
@@ -23643,7 +23641,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="154" spans="1:28" ht="53.65" customHeight="1">
+    <row r="154" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A154" s="10" t="s">
         <v>1365</v>
       </c>
@@ -23729,7 +23727,7 @@
         <v>2587</v>
       </c>
     </row>
-    <row r="155" spans="1:28" ht="53.65" customHeight="1">
+    <row r="155" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A155" s="10" t="s">
         <v>1365</v>
       </c>
@@ -23815,7 +23813,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="156" spans="1:28" ht="53.65" customHeight="1">
+    <row r="156" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A156" s="10" t="s">
         <v>1365</v>
       </c>
@@ -23901,7 +23899,7 @@
         <v>2587</v>
       </c>
     </row>
-    <row r="157" spans="1:28" ht="53.65" customHeight="1">
+    <row r="157" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A157" s="10" t="s">
         <v>1365</v>
       </c>
@@ -23987,7 +23985,7 @@
         <v>2587</v>
       </c>
     </row>
-    <row r="158" spans="1:28" ht="53.65" customHeight="1">
+    <row r="158" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A158" s="10" t="s">
         <v>1365</v>
       </c>
@@ -24073,7 +24071,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="159" spans="1:28" ht="53.65" customHeight="1">
+    <row r="159" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A159" s="10" t="s">
         <v>1365</v>
       </c>
@@ -24159,7 +24157,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="160" spans="1:28" ht="53.65" customHeight="1">
+    <row r="160" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A160" s="10" t="s">
         <v>1365</v>
       </c>
@@ -24245,7 +24243,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="161" spans="1:28" ht="53.65" customHeight="1">
+    <row r="161" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A161" s="10" t="s">
         <v>1365</v>
       </c>
@@ -24331,7 +24329,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="162" spans="1:28" ht="53.65" customHeight="1">
+    <row r="162" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A162" s="10" t="s">
         <v>1365</v>
       </c>
@@ -24417,7 +24415,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="163" spans="1:28" ht="53.65" customHeight="1">
+    <row r="163" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A163" s="10" t="s">
         <v>1365</v>
       </c>
@@ -24503,7 +24501,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="164" spans="1:28" ht="53.65" customHeight="1">
+    <row r="164" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A164" s="10" t="s">
         <v>1365</v>
       </c>
@@ -24589,7 +24587,7 @@
         <v>2590</v>
       </c>
     </row>
-    <row r="165" spans="1:28" ht="53.65" customHeight="1">
+    <row r="165" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A165" s="10" t="s">
         <v>1365</v>
       </c>
@@ -24675,7 +24673,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="166" spans="1:28" ht="53.65" customHeight="1">
+    <row r="166" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A166" s="10" t="s">
         <v>1365</v>
       </c>
@@ -24761,7 +24759,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="167" spans="1:28" ht="53.65" customHeight="1">
+    <row r="167" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A167" s="10" t="s">
         <v>1365</v>
       </c>
@@ -24847,7 +24845,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="168" spans="1:28" ht="53.65" customHeight="1">
+    <row r="168" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A168" s="10" t="s">
         <v>1365</v>
       </c>
@@ -24933,7 +24931,7 @@
         <v>2591</v>
       </c>
     </row>
-    <row r="169" spans="1:28" ht="53.65" customHeight="1">
+    <row r="169" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A169" s="10" t="s">
         <v>1365</v>
       </c>
@@ -25019,7 +25017,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="170" spans="1:28" ht="53.65" customHeight="1">
+    <row r="170" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A170" s="10" t="s">
         <v>1365</v>
       </c>
@@ -25105,7 +25103,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="171" spans="1:28" ht="53.65" customHeight="1">
+    <row r="171" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A171" s="10" t="s">
         <v>1365</v>
       </c>
@@ -25191,7 +25189,7 @@
         <v>2592</v>
       </c>
     </row>
-    <row r="172" spans="1:28" ht="53.65" customHeight="1">
+    <row r="172" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A172" s="10" t="s">
         <v>1365</v>
       </c>
@@ -25277,7 +25275,7 @@
         <v>2593</v>
       </c>
     </row>
-    <row r="173" spans="1:28" ht="53.65" customHeight="1">
+    <row r="173" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A173" s="10" t="s">
         <v>1365</v>
       </c>
@@ -25363,7 +25361,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="174" spans="1:28" ht="53.65" customHeight="1">
+    <row r="174" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A174" s="10" t="s">
         <v>1365</v>
       </c>
@@ -25449,7 +25447,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="175" spans="1:28" ht="53.65" customHeight="1">
+    <row r="175" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A175" s="10" t="s">
         <v>1365</v>
       </c>
@@ -25535,7 +25533,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="176" spans="1:28" ht="53.65" customHeight="1">
+    <row r="176" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A176" s="10" t="s">
         <v>1365</v>
       </c>
@@ -25621,7 +25619,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="177" spans="1:28" ht="53.65" customHeight="1">
+    <row r="177" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A177" s="10" t="s">
         <v>1365</v>
       </c>
@@ -25707,7 +25705,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="178" spans="1:28" ht="53.65" customHeight="1">
+    <row r="178" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A178" s="10" t="s">
         <v>1365</v>
       </c>
@@ -25793,7 +25791,7 @@
         <v>2594</v>
       </c>
     </row>
-    <row r="179" spans="1:28" ht="53.65" customHeight="1">
+    <row r="179" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A179" s="10" t="s">
         <v>1365</v>
       </c>
@@ -25879,7 +25877,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="180" spans="1:28" ht="53.65" customHeight="1">
+    <row r="180" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A180" s="11" t="s">
         <v>1679</v>
       </c>
@@ -25965,7 +25963,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="181" spans="1:28" ht="53.65" customHeight="1">
+    <row r="181" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A181" s="11" t="s">
         <v>1679</v>
       </c>
@@ -26051,7 +26049,7 @@
         <v>2595</v>
       </c>
     </row>
-    <row r="182" spans="1:28" ht="53.65" customHeight="1">
+    <row r="182" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A182" s="11" t="s">
         <v>1679</v>
       </c>
@@ -26137,7 +26135,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="183" spans="1:28" ht="53.65" customHeight="1">
+    <row r="183" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A183" s="11" t="s">
         <v>1679</v>
       </c>
@@ -26223,7 +26221,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="184" spans="1:28" ht="53.65" customHeight="1">
+    <row r="184" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A184" s="11" t="s">
         <v>1679</v>
       </c>
@@ -26309,7 +26307,7 @@
         <v>2595</v>
       </c>
     </row>
-    <row r="185" spans="1:28" ht="53.65" customHeight="1">
+    <row r="185" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A185" s="11" t="s">
         <v>1679</v>
       </c>
@@ -26395,7 +26393,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="186" spans="1:28" ht="53.65" customHeight="1">
+    <row r="186" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A186" s="11" t="s">
         <v>1679</v>
       </c>
@@ -26481,7 +26479,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="187" spans="1:28" ht="53.65" customHeight="1">
+    <row r="187" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A187" s="11" t="s">
         <v>1679</v>
       </c>
@@ -26567,7 +26565,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="188" spans="1:28" ht="53.65" customHeight="1">
+    <row r="188" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A188" s="11" t="s">
         <v>1679</v>
       </c>
@@ -26653,7 +26651,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="189" spans="1:28" ht="53.65" customHeight="1">
+    <row r="189" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A189" s="11" t="s">
         <v>1679</v>
       </c>
@@ -26739,7 +26737,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="190" spans="1:28" ht="53.65" customHeight="1">
+    <row r="190" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A190" s="11" t="s">
         <v>1679</v>
       </c>
@@ -26825,7 +26823,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="191" spans="1:28" ht="53.65" customHeight="1">
+    <row r="191" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A191" s="11" t="s">
         <v>1679</v>
       </c>
@@ -26911,7 +26909,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="192" spans="1:28" ht="53.65" customHeight="1">
+    <row r="192" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A192" s="11" t="s">
         <v>1679</v>
       </c>
@@ -26997,7 +26995,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="193" spans="1:28" ht="53.65" customHeight="1">
+    <row r="193" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A193" s="11" t="s">
         <v>1679</v>
       </c>
@@ -27083,7 +27081,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="194" spans="1:28" ht="53.65" customHeight="1">
+    <row r="194" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A194" s="11" t="s">
         <v>1679</v>
       </c>
@@ -27169,7 +27167,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="195" spans="1:28" ht="53.65" customHeight="1">
+    <row r="195" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A195" s="11" t="s">
         <v>1679</v>
       </c>
@@ -27255,7 +27253,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="196" spans="1:28" ht="53.65" customHeight="1">
+    <row r="196" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A196" s="11" t="s">
         <v>1679</v>
       </c>
@@ -27341,7 +27339,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="197" spans="1:28" ht="53.65" customHeight="1">
+    <row r="197" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A197" s="11" t="s">
         <v>1679</v>
       </c>
@@ -27427,7 +27425,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="198" spans="1:28" ht="53.65" customHeight="1">
+    <row r="198" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A198" s="11" t="s">
         <v>1679</v>
       </c>
@@ -27513,7 +27511,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="199" spans="1:28" ht="53.65" customHeight="1">
+    <row r="199" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A199" s="11" t="s">
         <v>1679</v>
       </c>
@@ -27599,7 +27597,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="200" spans="1:28" ht="53.65" customHeight="1">
+    <row r="200" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A200" s="11" t="s">
         <v>1679</v>
       </c>
@@ -27685,7 +27683,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="201" spans="1:28" ht="53.65" customHeight="1">
+    <row r="201" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A201" s="11" t="s">
         <v>1679</v>
       </c>
@@ -27771,7 +27769,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="202" spans="1:28" ht="53.65" customHeight="1">
+    <row r="202" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A202" s="11" t="s">
         <v>1679</v>
       </c>
@@ -27857,7 +27855,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="203" spans="1:28" ht="53.65" customHeight="1">
+    <row r="203" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A203" s="11" t="s">
         <v>1679</v>
       </c>
@@ -27943,7 +27941,7 @@
         <v>2597</v>
       </c>
     </row>
-    <row r="204" spans="1:28" ht="53.65" customHeight="1">
+    <row r="204" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A204" s="11" t="s">
         <v>1679</v>
       </c>
@@ -28029,7 +28027,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="205" spans="1:28" ht="53.65" customHeight="1">
+    <row r="205" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A205" s="11" t="s">
         <v>1679</v>
       </c>
@@ -28115,7 +28113,7 @@
         <v>2596</v>
       </c>
     </row>
-    <row r="206" spans="1:28" ht="53.65" customHeight="1">
+    <row r="206" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A206" s="11" t="s">
         <v>1679</v>
       </c>
@@ -28201,7 +28199,7 @@
         <v>2598</v>
       </c>
     </row>
-    <row r="207" spans="1:28" ht="53.65" customHeight="1">
+    <row r="207" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A207" s="11" t="s">
         <v>1679</v>
       </c>
@@ -28287,7 +28285,7 @@
         <v>2598</v>
       </c>
     </row>
-    <row r="208" spans="1:28" ht="53.65" customHeight="1">
+    <row r="208" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A208" s="11" t="s">
         <v>1679</v>
       </c>
@@ -28373,7 +28371,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="209" spans="1:28" ht="53.65" customHeight="1">
+    <row r="209" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A209" s="11" t="s">
         <v>1679</v>
       </c>
@@ -28459,7 +28457,7 @@
         <v>1319</v>
       </c>
     </row>
-    <row r="210" spans="1:28" ht="53.65" customHeight="1">
+    <row r="210" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A210" s="11" t="s">
         <v>1679</v>
       </c>
@@ -28545,7 +28543,7 @@
         <v>2599</v>
       </c>
     </row>
-    <row r="211" spans="1:28" ht="53.65" customHeight="1">
+    <row r="211" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A211" s="11" t="s">
         <v>1679</v>
       </c>
@@ -28631,7 +28629,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="212" spans="1:28" ht="53.65" customHeight="1">
+    <row r="212" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A212" s="11" t="s">
         <v>1679</v>
       </c>
@@ -28717,7 +28715,7 @@
         <v>2589</v>
       </c>
     </row>
-    <row r="213" spans="1:28" ht="53.65" customHeight="1">
+    <row r="213" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A213" s="11" t="s">
         <v>1679</v>
       </c>
@@ -28803,7 +28801,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="214" spans="1:28" ht="53.65" customHeight="1">
+    <row r="214" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A214" s="11" t="s">
         <v>1679</v>
       </c>
@@ -28889,7 +28887,7 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="215" spans="1:28" ht="53.65" customHeight="1">
+    <row r="215" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A215" s="12" t="s">
         <v>2002</v>
       </c>
@@ -28975,7 +28973,7 @@
         <v>2583</v>
       </c>
     </row>
-    <row r="216" spans="1:28" ht="53.65" customHeight="1">
+    <row r="216" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A216" s="12" t="s">
         <v>2002</v>
       </c>
@@ -29061,7 +29059,7 @@
         <v>2583</v>
       </c>
     </row>
-    <row r="217" spans="1:28" ht="53.65" customHeight="1">
+    <row r="217" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A217" s="12" t="s">
         <v>2002</v>
       </c>
@@ -29147,7 +29145,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="218" spans="1:28" ht="53.65" customHeight="1">
+    <row r="218" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A218" s="12" t="s">
         <v>2002</v>
       </c>
@@ -29233,7 +29231,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="219" spans="1:28" ht="53.65" customHeight="1">
+    <row r="219" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A219" s="12" t="s">
         <v>2002</v>
       </c>
@@ -29319,7 +29317,7 @@
         <v>2583</v>
       </c>
     </row>
-    <row r="220" spans="1:28" ht="53.65" customHeight="1">
+    <row r="220" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A220" s="12" t="s">
         <v>2002</v>
       </c>
@@ -29403,7 +29401,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="221" spans="1:28" ht="53.65" customHeight="1">
+    <row r="221" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A221" s="12" t="s">
         <v>2002</v>
       </c>
@@ -29489,7 +29487,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="222" spans="1:28" ht="53.65" customHeight="1">
+    <row r="222" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A222" s="12" t="s">
         <v>2002</v>
       </c>
@@ -29575,7 +29573,7 @@
         <v>1554</v>
       </c>
     </row>
-    <row r="223" spans="1:28" ht="53.65" customHeight="1">
+    <row r="223" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A223" s="12" t="s">
         <v>2002</v>
       </c>
@@ -29661,7 +29659,7 @@
         <v>1554</v>
       </c>
     </row>
-    <row r="224" spans="1:28" ht="53.65" customHeight="1">
+    <row r="224" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A224" s="12" t="s">
         <v>2002</v>
       </c>
@@ -29747,7 +29745,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="225" spans="1:28" ht="53.65" customHeight="1">
+    <row r="225" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A225" s="12" t="s">
         <v>2002</v>
       </c>
@@ -29833,7 +29831,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="226" spans="1:28" ht="53.65" customHeight="1">
+    <row r="226" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A226" s="12" t="s">
         <v>2002</v>
       </c>
@@ -29919,7 +29917,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="227" spans="1:28" ht="53.65" customHeight="1">
+    <row r="227" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A227" s="12" t="s">
         <v>2002</v>
       </c>
@@ -30005,7 +30003,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="228" spans="1:28" ht="53.65" customHeight="1">
+    <row r="228" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A228" s="12" t="s">
         <v>2002</v>
       </c>
@@ -30091,7 +30089,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="229" spans="1:28" ht="53.65" customHeight="1">
+    <row r="229" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A229" s="12" t="s">
         <v>2002</v>
       </c>
@@ -30177,7 +30175,7 @@
         <v>1554</v>
       </c>
     </row>
-    <row r="230" spans="1:28" ht="53.65" customHeight="1">
+    <row r="230" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A230" s="12" t="s">
         <v>2002</v>
       </c>
@@ -30263,7 +30261,7 @@
         <v>1554</v>
       </c>
     </row>
-    <row r="231" spans="1:28" ht="53.65" customHeight="1">
+    <row r="231" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A231" s="12" t="s">
         <v>2002</v>
       </c>
@@ -30349,7 +30347,7 @@
         <v>1554</v>
       </c>
     </row>
-    <row r="232" spans="1:28" ht="53.65" customHeight="1">
+    <row r="232" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A232" s="12" t="s">
         <v>2002</v>
       </c>
@@ -30435,7 +30433,7 @@
         <v>1554</v>
       </c>
     </row>
-    <row r="233" spans="1:28" ht="53.65" customHeight="1">
+    <row r="233" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A233" s="12" t="s">
         <v>2002</v>
       </c>
@@ -30521,7 +30519,7 @@
         <v>1554</v>
       </c>
     </row>
-    <row r="234" spans="1:28" ht="53.65" customHeight="1">
+    <row r="234" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A234" s="12" t="s">
         <v>2002</v>
       </c>
@@ -30607,7 +30605,7 @@
         <v>1554</v>
       </c>
     </row>
-    <row r="235" spans="1:28" ht="53.65" customHeight="1">
+    <row r="235" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A235" s="12" t="s">
         <v>2002</v>
       </c>
@@ -30693,7 +30691,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="236" spans="1:28" ht="53.65" customHeight="1">
+    <row r="236" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A236" s="12" t="s">
         <v>2002</v>
       </c>
@@ -30779,7 +30777,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="237" spans="1:28" ht="53.65" customHeight="1">
+    <row r="237" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A237" s="12" t="s">
         <v>2002</v>
       </c>
@@ -30865,7 +30863,7 @@
         <v>1554</v>
       </c>
     </row>
-    <row r="238" spans="1:28" ht="53.65" customHeight="1">
+    <row r="238" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A238" s="12" t="s">
         <v>2002</v>
       </c>
@@ -30951,7 +30949,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="239" spans="1:28" ht="53.65" customHeight="1">
+    <row r="239" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A239" s="12" t="s">
         <v>2002</v>
       </c>
@@ -31037,7 +31035,7 @@
         <v>1554</v>
       </c>
     </row>
-    <row r="240" spans="1:28" ht="53.65" customHeight="1">
+    <row r="240" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A240" s="12" t="s">
         <v>2002</v>
       </c>
@@ -31123,7 +31121,7 @@
         <v>1554</v>
       </c>
     </row>
-    <row r="241" spans="1:28" ht="53.65" customHeight="1">
+    <row r="241" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A241" s="12" t="s">
         <v>2002</v>
       </c>
@@ -31209,7 +31207,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="242" spans="1:28" ht="53.65" customHeight="1">
+    <row r="242" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A242" s="12" t="s">
         <v>2002</v>
       </c>
@@ -31295,7 +31293,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="243" spans="1:28" ht="53.65" customHeight="1">
+    <row r="243" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A243" s="12" t="s">
         <v>2002</v>
       </c>
@@ -31381,7 +31379,7 @@
         <v>1554</v>
       </c>
     </row>
-    <row r="244" spans="1:28" ht="53.65" customHeight="1">
+    <row r="244" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A244" s="12" t="s">
         <v>2002</v>
       </c>
@@ -31467,7 +31465,7 @@
         <v>1554</v>
       </c>
     </row>
-    <row r="245" spans="1:28" ht="53.65" customHeight="1">
+    <row r="245" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A245" s="12" t="s">
         <v>2002</v>
       </c>
@@ -31553,7 +31551,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="246" spans="1:28" ht="53.65" customHeight="1">
+    <row r="246" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A246" s="12" t="s">
         <v>2002</v>
       </c>
@@ -31639,7 +31637,7 @@
         <v>1554</v>
       </c>
     </row>
-    <row r="247" spans="1:28" ht="53.65" customHeight="1">
+    <row r="247" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A247" s="12" t="s">
         <v>2002</v>
       </c>
@@ -31725,7 +31723,7 @@
         <v>1554</v>
       </c>
     </row>
-    <row r="248" spans="1:28" ht="53.65" customHeight="1">
+    <row r="248" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A248" s="12" t="s">
         <v>2002</v>
       </c>
@@ -31811,7 +31809,7 @@
         <v>1554</v>
       </c>
     </row>
-    <row r="249" spans="1:28" ht="53.65" customHeight="1">
+    <row r="249" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A249" s="12" t="s">
         <v>2002</v>
       </c>
@@ -31897,7 +31895,7 @@
         <v>2602</v>
       </c>
     </row>
-    <row r="250" spans="1:28" ht="53.65" customHeight="1">
+    <row r="250" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A250" s="13" t="s">
         <v>2277</v>
       </c>
@@ -31983,7 +31981,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="251" spans="1:28" ht="53.65" customHeight="1">
+    <row r="251" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A251" s="13" t="s">
         <v>2277</v>
       </c>
@@ -32069,7 +32067,7 @@
         <v>2604</v>
       </c>
     </row>
-    <row r="252" spans="1:28" ht="53.65" customHeight="1">
+    <row r="252" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A252" s="13" t="s">
         <v>2277</v>
       </c>
@@ -32155,7 +32153,7 @@
         <v>2117</v>
       </c>
     </row>
-    <row r="253" spans="1:28" ht="53.65" customHeight="1">
+    <row r="253" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A253" s="13" t="s">
         <v>2277</v>
       </c>
@@ -32241,7 +32239,7 @@
         <v>2117</v>
       </c>
     </row>
-    <row r="254" spans="1:28" ht="53.65" customHeight="1">
+    <row r="254" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A254" s="13" t="s">
         <v>2277</v>
       </c>
@@ -32327,7 +32325,7 @@
         <v>2604</v>
       </c>
     </row>
-    <row r="255" spans="1:28" ht="53.65" customHeight="1">
+    <row r="255" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A255" s="13" t="s">
         <v>2277</v>
       </c>
@@ -32413,7 +32411,7 @@
         <v>2594</v>
       </c>
     </row>
-    <row r="256" spans="1:28" ht="53.65" customHeight="1">
+    <row r="256" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A256" s="13" t="s">
         <v>2277</v>
       </c>
@@ -32499,7 +32497,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="257" spans="1:28" ht="53.65" customHeight="1">
+    <row r="257" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A257" s="13" t="s">
         <v>2277</v>
       </c>
@@ -32585,7 +32583,7 @@
         <v>2594</v>
       </c>
     </row>
-    <row r="258" spans="1:28" ht="53.65" customHeight="1">
+    <row r="258" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A258" s="13" t="s">
         <v>2277</v>
       </c>
@@ -32671,7 +32669,7 @@
         <v>2594</v>
       </c>
     </row>
-    <row r="259" spans="1:28" ht="53.65" customHeight="1">
+    <row r="259" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A259" s="13" t="s">
         <v>2277</v>
       </c>
@@ -32757,7 +32755,7 @@
         <v>2117</v>
       </c>
     </row>
-    <row r="260" spans="1:28" ht="53.65" customHeight="1">
+    <row r="260" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A260" s="13" t="s">
         <v>2277</v>
       </c>
@@ -32843,7 +32841,7 @@
         <v>2117</v>
       </c>
     </row>
-    <row r="261" spans="1:28" ht="53.65" customHeight="1">
+    <row r="261" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A261" s="13" t="s">
         <v>2277</v>
       </c>
@@ -32929,7 +32927,7 @@
         <v>2117</v>
       </c>
     </row>
-    <row r="262" spans="1:28" ht="53.65" customHeight="1">
+    <row r="262" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A262" s="13" t="s">
         <v>2277</v>
       </c>
@@ -33015,7 +33013,7 @@
         <v>2117</v>
       </c>
     </row>
-    <row r="263" spans="1:28" ht="53.65" customHeight="1">
+    <row r="263" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A263" s="13" t="s">
         <v>2277</v>
       </c>
@@ -33101,7 +33099,7 @@
         <v>2117</v>
       </c>
     </row>
-    <row r="264" spans="1:28" ht="53.65" customHeight="1">
+    <row r="264" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A264" s="13" t="s">
         <v>2277</v>
       </c>
@@ -33187,7 +33185,7 @@
         <v>2594</v>
       </c>
     </row>
-    <row r="265" spans="1:28" ht="53.65" customHeight="1">
+    <row r="265" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A265" s="13" t="s">
         <v>2277</v>
       </c>
@@ -33273,7 +33271,7 @@
         <v>2594</v>
       </c>
     </row>
-    <row r="266" spans="1:28" ht="53.65" customHeight="1">
+    <row r="266" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A266" s="13" t="s">
         <v>2277</v>
       </c>
@@ -33359,7 +33357,7 @@
         <v>2594</v>
       </c>
     </row>
-    <row r="267" spans="1:28" ht="53.65" customHeight="1">
+    <row r="267" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A267" s="13" t="s">
         <v>2277</v>
       </c>
@@ -33445,7 +33443,7 @@
         <v>2594</v>
       </c>
     </row>
-    <row r="268" spans="1:28" ht="53.65" customHeight="1">
+    <row r="268" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A268" s="13" t="s">
         <v>2277</v>
       </c>
@@ -33531,7 +33529,7 @@
         <v>2594</v>
       </c>
     </row>
-    <row r="269" spans="1:28" ht="53.65" customHeight="1">
+    <row r="269" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A269" s="13" t="s">
         <v>2277</v>
       </c>
@@ -33617,7 +33615,7 @@
         <v>2450</v>
       </c>
     </row>
-    <row r="270" spans="1:28" ht="53.65" customHeight="1">
+    <row r="270" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A270" s="13" t="s">
         <v>2277</v>
       </c>
@@ -33703,7 +33701,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="271" spans="1:28" ht="53.65" customHeight="1">
+    <row r="271" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A271" s="13" t="s">
         <v>2277</v>
       </c>
@@ -33789,7 +33787,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="272" spans="1:28" ht="53.65" customHeight="1">
+    <row r="272" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A272" s="13" t="s">
         <v>2277</v>
       </c>
@@ -33875,7 +33873,7 @@
         <v>2450</v>
       </c>
     </row>
-    <row r="273" spans="1:28" ht="53.65" customHeight="1">
+    <row r="273" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A273" s="13" t="s">
         <v>2277</v>
       </c>
@@ -33961,7 +33959,7 @@
         <v>2605</v>
       </c>
     </row>
-    <row r="274" spans="1:28" ht="53.65" customHeight="1">
+    <row r="274" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A274" s="13" t="s">
         <v>2277</v>
       </c>
@@ -34047,7 +34045,7 @@
         <v>2450</v>
       </c>
     </row>
-    <row r="275" spans="1:28" ht="53.65" customHeight="1">
+    <row r="275" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A275" s="13" t="s">
         <v>2277</v>
       </c>
@@ -34133,7 +34131,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="276" spans="1:28" ht="53.65" customHeight="1">
+    <row r="276" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A276" s="13" t="s">
         <v>2277</v>
       </c>
@@ -34219,7 +34217,7 @@
         <v>1291</v>
       </c>
     </row>
-    <row r="277" spans="1:28" ht="53.65" customHeight="1">
+    <row r="277" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A277" s="13" t="s">
         <v>2277</v>
       </c>
@@ -34305,7 +34303,7 @@
         <v>2450</v>
       </c>
     </row>
-    <row r="278" spans="1:28" ht="53.65" customHeight="1">
+    <row r="278" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A278" s="13" t="s">
         <v>2277</v>
       </c>
@@ -34391,7 +34389,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="279" spans="1:28" ht="53.65" customHeight="1">
+    <row r="279" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A279" s="13" t="s">
         <v>2277</v>
       </c>
@@ -34477,7 +34475,7 @@
         <v>2450</v>
       </c>
     </row>
-    <row r="280" spans="1:28" ht="53.65" customHeight="1">
+    <row r="280" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A280" s="13" t="s">
         <v>2277</v>
       </c>
@@ -34563,7 +34561,7 @@
         <v>2450</v>
       </c>
     </row>
-    <row r="281" spans="1:28" ht="53.65" customHeight="1">
+    <row r="281" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A281" s="13" t="s">
         <v>2277</v>
       </c>
@@ -34649,7 +34647,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="282" spans="1:28" ht="53.65" customHeight="1">
+    <row r="282" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A282" s="13" t="s">
         <v>2277</v>
       </c>
@@ -34735,7 +34733,7 @@
         <v>2594</v>
       </c>
     </row>
-    <row r="283" spans="1:28" ht="53.65" customHeight="1">
+    <row r="283" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A283" s="13" t="s">
         <v>2277</v>
       </c>
@@ -34821,7 +34819,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="284" spans="1:28" ht="53.65" customHeight="1">
+    <row r="284" spans="1:28" ht="53.65" hidden="1" customHeight="1">
       <c r="A284" s="13" t="s">
         <v>2277</v>
       </c>
@@ -52640,18 +52638,19 @@
       <c r="X1248" s="14"/>
     </row>
   </sheetData>
+  <autoFilter ref="A4:AB284" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="7">
+      <filters>
+        <filter val="Change in climagte extremes"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:AB284">
     <sortCondition ref="A5:A284"/>
     <sortCondition ref="B5:B284"/>
     <sortCondition ref="C5:C284"/>
   </sortState>
   <mergeCells count="16">
-    <mergeCell ref="Y1:AB1"/>
-    <mergeCell ref="Y2:Z3"/>
-    <mergeCell ref="AA2:AB3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="S2:U3"/>
-    <mergeCell ref="R2:R3"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="W1:X1"/>
     <mergeCell ref="D1:H1"/>
@@ -52662,6 +52661,12 @@
     <mergeCell ref="I1:R1"/>
     <mergeCell ref="S1:V1"/>
     <mergeCell ref="F3:G3"/>
+    <mergeCell ref="Y1:AB1"/>
+    <mergeCell ref="Y2:Z3"/>
+    <mergeCell ref="AA2:AB3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="S2:U3"/>
+    <mergeCell ref="R2:R3"/>
   </mergeCells>
   <conditionalFormatting sqref="D14:D18">
     <cfRule type="cellIs" dxfId="19" priority="6" operator="equal">
@@ -53015,6 +53020,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="9c70d178-d21c-48a3-aa0e-ddb58e3b7295">
@@ -53025,15 +53039,6 @@
     <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -53057,6 +53062,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4CC43FB1-6F13-4FC9-A3DC-D5E732E9F9F7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{32E97209-EA28-4125-8A8D-2BD814449A59}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -53066,12 +53079,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4CC43FB1-6F13-4FC9-A3DC-D5E732E9F9F7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>